<commit_message>
R anlaysis comments highlights and improvement. More elaborations on R residual interpretations.
</commit_message>
<xml_diff>
--- a/data/snb-target rate-policy rate-2000-2025.xlsx
+++ b/data/snb-target rate-policy rate-2000-2025.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dongyuangao/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/407a39b4e6a633f5/文档/学业/硕士hslu/Lectures Lessons Subjects/Time series analysis/project/R git/time_series_project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2892866F-C468-0A45-BBDC-5D5CFEAF402C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{2892866F-C468-0A45-BBDC-5D5CFEAF402C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E32924D5-7617-E743-8512-F62794C9FDDC}"/>
   <bookViews>
-    <workbookView xWindow="3400" yWindow="10580" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8440" yWindow="1060" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1436,8 +1449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K320"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="116" workbookViewId="0">
+      <selection activeCell="B125" sqref="B125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2178,6 +2191,10 @@
       <c r="A37" t="s">
         <v>55</v>
       </c>
+      <c r="B37">
+        <f>(C37+D37)/2</f>
+        <v>3.25</v>
+      </c>
       <c r="C37">
         <v>2.75</v>
       </c>
@@ -2207,6 +2224,10 @@
       <c r="A38" t="s">
         <v>56</v>
       </c>
+      <c r="B38">
+        <f>(C38+D38)/2</f>
+        <v>2.25</v>
+      </c>
       <c r="C38">
         <v>1.75</v>
       </c>
@@ -4765,6 +4786,10 @@
       <c r="A123" t="s">
         <v>141</v>
       </c>
+      <c r="B123">
+        <f>(C123+D123)/2</f>
+        <v>2.5</v>
+      </c>
       <c r="C123">
         <v>2</v>
       </c>
@@ -4796,6 +4821,10 @@
     <row r="124" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>142</v>
+      </c>
+      <c r="B124">
+        <f>(C124+D124)/2</f>
+        <v>1</v>
       </c>
       <c r="C124">
         <v>0.5</v>

</xml_diff>